<commit_message>
Analysis KnowledgeStore with manually annotated MeanTime corpus
</commit_message>
<xml_diff>
--- a/Data, experiments, analyses/WikiNews_analysis_ESO.xlsx
+++ b/Data, experiments, analyses/WikiNews_analysis_ESO.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24800" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="600" yWindow="0" windowWidth="24800" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="381">
   <si>
     <t>predicate</t>
   </si>
@@ -913,6 +913,255 @@
   </si>
   <si>
     <t>Number of events with this issue (note that multiple issues can pertain to one event):</t>
+  </si>
+  <si>
+    <t>ev 4</t>
+  </si>
+  <si>
+    <t>62929_A380_makes_maiden_flight_to_US.xml.naf</t>
+  </si>
+  <si>
+    <t>land</t>
+  </si>
+  <si>
+    <t>238039_Apple_Inc_CEO_Steve.xml.naf</t>
+  </si>
+  <si>
+    <t>transplant</t>
+  </si>
+  <si>
+    <t>ev 19</t>
+  </si>
+  <si>
+    <t>Damaging</t>
+  </si>
+  <si>
+    <t>71526_Aeroflot_negotiates_purchase_of_22_new_Boeing_787_Dreamliner_aircraft.xml.naf</t>
+  </si>
+  <si>
+    <t>ev 15</t>
+  </si>
+  <si>
+    <t>Buying, BeingInuse</t>
+  </si>
+  <si>
+    <t>purchase</t>
+  </si>
+  <si>
+    <t>ev 6</t>
+  </si>
+  <si>
+    <t>two classes generated where it should have been one</t>
+  </si>
+  <si>
+    <t>108294_Government_Accountability_Office_requests_rerun_of_US_Air_Force_tanker_bid.xml.na</t>
+  </si>
+  <si>
+    <t>114864_Global_markets_plunge.xml.naf</t>
+  </si>
+  <si>
+    <t>ev 13</t>
+  </si>
+  <si>
+    <t>115711_Asian_stock_markets_slide.xml.naf</t>
+  </si>
+  <si>
+    <t>ask (?!)</t>
+  </si>
+  <si>
+    <t>NP structure, no idea why predicate 'ask' is here</t>
+  </si>
+  <si>
+    <t>112579_Dow_falls_340_points_amid_unemployment_and_retail_sales_rates_news.xml.na</t>
+  </si>
+  <si>
+    <t>ev 5</t>
+  </si>
+  <si>
+    <t>Increasing, Decreasing</t>
+  </si>
+  <si>
+    <t>decrease, drop, fall</t>
+  </si>
+  <si>
+    <t>NAF2SEM error (mixed up predicates and role)</t>
+  </si>
+  <si>
+    <t>114719_Markets_down_across_the_world.xml.naf</t>
+  </si>
+  <si>
+    <t>ev 18</t>
+  </si>
+  <si>
+    <t>fell</t>
+  </si>
+  <si>
+    <t>126878_Bankruptcy_for_U.S._automaker_GM_becomes_almost_certain_after_bondholder_offers_fail.xml.naf</t>
+  </si>
+  <si>
+    <t>Destroying</t>
+  </si>
+  <si>
+    <t>113278_Markets_rally_as_world_central_banks_infuse_cash.xml.naf</t>
+  </si>
+  <si>
+    <t>ev 39</t>
+  </si>
+  <si>
+    <t>FinancialTransaction</t>
+  </si>
+  <si>
+    <t>closures</t>
+  </si>
+  <si>
+    <t>pump</t>
+  </si>
+  <si>
+    <t>02977_Airbus_parent_EADS_wins_13_billion_UK_RAF_airtanker_contract.xml.naf</t>
+  </si>
+  <si>
+    <t>win, won, wins</t>
+  </si>
+  <si>
+    <t>199629_Apple_executive_leaves_company.xml.naf</t>
+  </si>
+  <si>
+    <t>ev 24</t>
+  </si>
+  <si>
+    <t>received</t>
+  </si>
+  <si>
+    <t>ev 14</t>
+  </si>
+  <si>
+    <t>107785_Apple_launches_3G.xml.naf</t>
+  </si>
+  <si>
+    <t>118147_US_automaker_bailout_deal_fails_to_pass_Senate.xml.naf</t>
+  </si>
+  <si>
+    <t>ev 25</t>
+  </si>
+  <si>
+    <t>141225_British_FTSE_index_reaches_one-year_high,_other_European_markets_rise.xml.naf</t>
+  </si>
+  <si>
+    <t>increased</t>
+  </si>
+  <si>
+    <t>87805_Indonesia_transport_minister.xml</t>
+  </si>
+  <si>
+    <t>ev 11</t>
+  </si>
+  <si>
+    <t>Killing</t>
+  </si>
+  <si>
+    <t>killed</t>
+  </si>
+  <si>
+    <t>Leaving</t>
+  </si>
+  <si>
+    <t>78496_Airbus_A380_test_flight_delayed_after_accident.xml.naf</t>
+  </si>
+  <si>
+    <t>ev 29</t>
+  </si>
+  <si>
+    <t>leaving</t>
+  </si>
+  <si>
+    <t>8951_World_largest_passenger_airliner_makes_first_flight.xml.naf</t>
+  </si>
+  <si>
+    <t>ev 1</t>
+  </si>
+  <si>
+    <t>lifting off, take-off</t>
+  </si>
+  <si>
+    <t>27227_Barack_Obama_presents_rescue_plan_after_GM_declaration_of_bankruptcy.xml.naf</t>
+  </si>
+  <si>
+    <t>ev 23</t>
+  </si>
+  <si>
+    <t>Lending</t>
+  </si>
+  <si>
+    <t>loaning</t>
+  </si>
+  <si>
+    <t>106653_Boeing_pushes_back_737_replacement_development.xml.naf</t>
+  </si>
+  <si>
+    <t>merged</t>
+  </si>
+  <si>
+    <t>129865_Airbus_offers_funding_to_search_for_black_boxes_from_Air_France_disaster.xml.naf</t>
+  </si>
+  <si>
+    <t>ev 20</t>
+  </si>
+  <si>
+    <t>contribute, offer, contribution</t>
+  </si>
+  <si>
+    <t>1173_Internal_emails_expose_Boeing-Air_Force_contract_discussions.xml.naf</t>
+  </si>
+  <si>
+    <t>160257_Ford_US_auto_sales_spike.xml.naf</t>
+  </si>
+  <si>
+    <t>ev 9</t>
+  </si>
+  <si>
+    <t>sold</t>
+  </si>
+  <si>
+    <t>KS-2 RESULTS BASED ON MANUALLY ANNOTATED MEANTIME CORPUS</t>
+  </si>
+  <si>
+    <t>1007169_Mary_Barra_appointed_as_General_Motors_chief.xml.naf</t>
+  </si>
+  <si>
+    <t>BeingLeader</t>
+  </si>
+  <si>
+    <t>lead</t>
+  </si>
+  <si>
+    <t>112579_Dow_falls_340_points_amid_unemployment_and_retail_sales_rates_news.xml.naf</t>
+  </si>
+  <si>
+    <t>ev 31</t>
+  </si>
+  <si>
+    <t>used</t>
+  </si>
+  <si>
+    <t>115064_Global_markets_surge_in_value.xml.naf</t>
+  </si>
+  <si>
+    <t>meeting</t>
+  </si>
+  <si>
+    <t>4764_Boeing_unveils_long-range_777.xml.naf</t>
+  </si>
+  <si>
+    <t>giving</t>
+  </si>
+  <si>
+    <t>37961_Apple_releases_program.xml.naf</t>
+  </si>
+  <si>
+    <t>BeingOperational</t>
+  </si>
+  <si>
+    <t>works</t>
   </si>
 </sst>
 </file>
@@ -960,7 +1209,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1048,8 +1297,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="35">
+  <cellStyleXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1085,8 +1371,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -1123,8 +1413,11 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="35">
+  <cellStyles count="39">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1142,6 +1435,8 @@
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1159,6 +1454,8 @@
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1488,10 +1785,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L79"/>
+  <dimension ref="A1:L114"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="K63" sqref="K63"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="C110" sqref="C110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3550,6 +3847,918 @@
     <row r="79" spans="1:10">
       <c r="A79" s="1"/>
     </row>
+    <row r="80" spans="1:10">
+      <c r="A80" s="22" t="s">
+        <v>367</v>
+      </c>
+      <c r="B80" s="23"/>
+      <c r="C80" s="24"/>
+    </row>
+    <row r="82" spans="1:12" s="1" customFormat="1">
+      <c r="A82" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H82" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I82" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J82" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="K82" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L82" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12">
+      <c r="A84" t="s">
+        <v>86</v>
+      </c>
+      <c r="B84" t="s">
+        <v>299</v>
+      </c>
+      <c r="D84" t="s">
+        <v>298</v>
+      </c>
+      <c r="E84" t="s">
+        <v>8</v>
+      </c>
+      <c r="F84" t="s">
+        <v>5</v>
+      </c>
+      <c r="G84" t="s">
+        <v>300</v>
+      </c>
+      <c r="H84" t="s">
+        <v>5</v>
+      </c>
+      <c r="I84" t="s">
+        <v>5</v>
+      </c>
+      <c r="K84" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12">
+      <c r="A85" t="s">
+        <v>37</v>
+      </c>
+      <c r="B85" t="s">
+        <v>301</v>
+      </c>
+      <c r="D85" t="s">
+        <v>303</v>
+      </c>
+      <c r="E85" t="s">
+        <v>304</v>
+      </c>
+      <c r="F85" t="s">
+        <v>5</v>
+      </c>
+      <c r="G85" t="s">
+        <v>302</v>
+      </c>
+      <c r="H85" t="s">
+        <v>5</v>
+      </c>
+      <c r="I85" t="s">
+        <v>5</v>
+      </c>
+      <c r="K85" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12">
+      <c r="A86" t="s">
+        <v>86</v>
+      </c>
+      <c r="B86" t="s">
+        <v>305</v>
+      </c>
+      <c r="D86" t="s">
+        <v>306</v>
+      </c>
+      <c r="E86" t="s">
+        <v>307</v>
+      </c>
+      <c r="F86" t="s">
+        <v>74</v>
+      </c>
+      <c r="G86" t="s">
+        <v>308</v>
+      </c>
+      <c r="H86" t="s">
+        <v>5</v>
+      </c>
+      <c r="I86" t="s">
+        <v>5</v>
+      </c>
+      <c r="K86" t="s">
+        <v>5</v>
+      </c>
+      <c r="L86" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12">
+      <c r="A87" t="s">
+        <v>1</v>
+      </c>
+      <c r="B87" t="s">
+        <v>108</v>
+      </c>
+      <c r="D87" t="s">
+        <v>309</v>
+      </c>
+      <c r="E87" t="s">
+        <v>23</v>
+      </c>
+      <c r="F87" t="s">
+        <v>5</v>
+      </c>
+      <c r="G87" t="s">
+        <v>30</v>
+      </c>
+      <c r="H87" t="s">
+        <v>5</v>
+      </c>
+      <c r="I87" t="s">
+        <v>5</v>
+      </c>
+      <c r="K87" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12">
+      <c r="A88" t="s">
+        <v>86</v>
+      </c>
+      <c r="B88" t="s">
+        <v>311</v>
+      </c>
+      <c r="D88" t="s">
+        <v>303</v>
+      </c>
+      <c r="E88" t="s">
+        <v>38</v>
+      </c>
+      <c r="F88" t="s">
+        <v>5</v>
+      </c>
+      <c r="G88" t="s">
+        <v>43</v>
+      </c>
+      <c r="H88" t="s">
+        <v>5</v>
+      </c>
+      <c r="I88" t="s">
+        <v>5</v>
+      </c>
+      <c r="K88" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12">
+      <c r="A89" t="s">
+        <v>1</v>
+      </c>
+      <c r="B89" t="s">
+        <v>312</v>
+      </c>
+      <c r="D89" t="s">
+        <v>313</v>
+      </c>
+      <c r="E89" t="s">
+        <v>304</v>
+      </c>
+      <c r="F89" t="s">
+        <v>5</v>
+      </c>
+      <c r="G89" t="s">
+        <v>48</v>
+      </c>
+      <c r="H89" t="s">
+        <v>5</v>
+      </c>
+      <c r="I89" t="s">
+        <v>5</v>
+      </c>
+      <c r="K89" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12">
+      <c r="A90" t="s">
+        <v>1</v>
+      </c>
+      <c r="B90" t="s">
+        <v>314</v>
+      </c>
+      <c r="D90" t="s">
+        <v>303</v>
+      </c>
+      <c r="E90" t="s">
+        <v>304</v>
+      </c>
+      <c r="F90" t="s">
+        <v>5</v>
+      </c>
+      <c r="G90" t="s">
+        <v>315</v>
+      </c>
+      <c r="H90" t="s">
+        <v>5</v>
+      </c>
+      <c r="I90" t="s">
+        <v>5</v>
+      </c>
+      <c r="K90" t="s">
+        <v>5</v>
+      </c>
+      <c r="L90" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12">
+      <c r="A91" t="s">
+        <v>1</v>
+      </c>
+      <c r="B91" t="s">
+        <v>317</v>
+      </c>
+      <c r="D91" t="s">
+        <v>318</v>
+      </c>
+      <c r="E91" t="s">
+        <v>319</v>
+      </c>
+      <c r="F91" t="s">
+        <v>3</v>
+      </c>
+      <c r="G91" t="s">
+        <v>320</v>
+      </c>
+      <c r="H91" t="s">
+        <v>3</v>
+      </c>
+      <c r="I91" t="s">
+        <v>3</v>
+      </c>
+      <c r="K91" t="s">
+        <v>5</v>
+      </c>
+      <c r="L91" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12">
+      <c r="A92" t="s">
+        <v>1</v>
+      </c>
+      <c r="B92" t="s">
+        <v>322</v>
+      </c>
+      <c r="D92" t="s">
+        <v>323</v>
+      </c>
+      <c r="E92" t="s">
+        <v>65</v>
+      </c>
+      <c r="F92" t="s">
+        <v>5</v>
+      </c>
+      <c r="G92" t="s">
+        <v>324</v>
+      </c>
+      <c r="H92" t="s">
+        <v>5</v>
+      </c>
+      <c r="I92" t="s">
+        <v>5</v>
+      </c>
+      <c r="K92" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12">
+      <c r="A93" t="s">
+        <v>18</v>
+      </c>
+      <c r="B93" t="s">
+        <v>325</v>
+      </c>
+      <c r="D93" t="s">
+        <v>303</v>
+      </c>
+      <c r="E93" t="s">
+        <v>326</v>
+      </c>
+      <c r="F93" t="s">
+        <v>5</v>
+      </c>
+      <c r="G93" t="s">
+        <v>330</v>
+      </c>
+      <c r="H93" t="s">
+        <v>5</v>
+      </c>
+      <c r="I93" t="s">
+        <v>5</v>
+      </c>
+      <c r="K93" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12">
+      <c r="A94" t="s">
+        <v>1</v>
+      </c>
+      <c r="B94" t="s">
+        <v>327</v>
+      </c>
+      <c r="D94" t="s">
+        <v>328</v>
+      </c>
+      <c r="E94" t="s">
+        <v>329</v>
+      </c>
+      <c r="F94" t="s">
+        <v>5</v>
+      </c>
+      <c r="G94" t="s">
+        <v>331</v>
+      </c>
+      <c r="H94" t="s">
+        <v>5</v>
+      </c>
+      <c r="I94" t="s">
+        <v>5</v>
+      </c>
+      <c r="K94" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12">
+      <c r="A95" t="s">
+        <v>86</v>
+      </c>
+      <c r="B95" t="s">
+        <v>332</v>
+      </c>
+      <c r="D95" t="s">
+        <v>335</v>
+      </c>
+      <c r="E95" t="s">
+        <v>93</v>
+      </c>
+      <c r="F95" t="s">
+        <v>5</v>
+      </c>
+      <c r="G95" t="s">
+        <v>333</v>
+      </c>
+      <c r="H95" t="s">
+        <v>5</v>
+      </c>
+      <c r="I95" t="s">
+        <v>5</v>
+      </c>
+      <c r="K95" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12">
+      <c r="A96" t="s">
+        <v>37</v>
+      </c>
+      <c r="B96" t="s">
+        <v>334</v>
+      </c>
+      <c r="D96" t="s">
+        <v>303</v>
+      </c>
+      <c r="E96" t="s">
+        <v>93</v>
+      </c>
+      <c r="F96" t="s">
+        <v>5</v>
+      </c>
+      <c r="G96" t="s">
+        <v>336</v>
+      </c>
+      <c r="H96" t="s">
+        <v>5</v>
+      </c>
+      <c r="I96" t="s">
+        <v>5</v>
+      </c>
+      <c r="K96" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11">
+      <c r="A97" t="s">
+        <v>37</v>
+      </c>
+      <c r="B97" t="s">
+        <v>338</v>
+      </c>
+      <c r="D97" t="s">
+        <v>337</v>
+      </c>
+      <c r="E97" t="s">
+        <v>97</v>
+      </c>
+      <c r="F97" t="s">
+        <v>5</v>
+      </c>
+      <c r="G97" t="s">
+        <v>98</v>
+      </c>
+      <c r="H97" t="s">
+        <v>5</v>
+      </c>
+      <c r="I97" t="s">
+        <v>5</v>
+      </c>
+      <c r="K97" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11">
+      <c r="A98" t="s">
+        <v>18</v>
+      </c>
+      <c r="B98" t="s">
+        <v>339</v>
+      </c>
+      <c r="D98" t="s">
+        <v>340</v>
+      </c>
+      <c r="E98" t="s">
+        <v>106</v>
+      </c>
+      <c r="F98" t="s">
+        <v>5</v>
+      </c>
+      <c r="G98" t="s">
+        <v>113</v>
+      </c>
+      <c r="H98" t="s">
+        <v>5</v>
+      </c>
+      <c r="I98" t="s">
+        <v>5</v>
+      </c>
+      <c r="K98" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11">
+      <c r="A99" t="s">
+        <v>1</v>
+      </c>
+      <c r="B99" t="s">
+        <v>341</v>
+      </c>
+      <c r="D99" t="s">
+        <v>323</v>
+      </c>
+      <c r="E99" t="s">
+        <v>106</v>
+      </c>
+      <c r="F99" t="s">
+        <v>5</v>
+      </c>
+      <c r="G99" t="s">
+        <v>342</v>
+      </c>
+      <c r="H99" t="s">
+        <v>5</v>
+      </c>
+      <c r="I99" t="s">
+        <v>5</v>
+      </c>
+      <c r="K99" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11">
+      <c r="A100" t="s">
+        <v>86</v>
+      </c>
+      <c r="B100" t="s">
+        <v>343</v>
+      </c>
+      <c r="D100" t="s">
+        <v>344</v>
+      </c>
+      <c r="E100" t="s">
+        <v>345</v>
+      </c>
+      <c r="F100" t="s">
+        <v>5</v>
+      </c>
+      <c r="G100" t="s">
+        <v>346</v>
+      </c>
+      <c r="H100" t="s">
+        <v>5</v>
+      </c>
+      <c r="I100" t="s">
+        <v>5</v>
+      </c>
+      <c r="K100" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11">
+      <c r="A101" t="s">
+        <v>86</v>
+      </c>
+      <c r="B101" t="s">
+        <v>348</v>
+      </c>
+      <c r="D101" t="s">
+        <v>349</v>
+      </c>
+      <c r="E101" t="s">
+        <v>347</v>
+      </c>
+      <c r="F101" t="s">
+        <v>5</v>
+      </c>
+      <c r="G101" t="s">
+        <v>350</v>
+      </c>
+      <c r="H101" t="s">
+        <v>5</v>
+      </c>
+      <c r="I101" t="s">
+        <v>5</v>
+      </c>
+      <c r="K101" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11">
+      <c r="A102" t="s">
+        <v>86</v>
+      </c>
+      <c r="B102" t="s">
+        <v>351</v>
+      </c>
+      <c r="D102" t="s">
+        <v>352</v>
+      </c>
+      <c r="E102" t="s">
+        <v>347</v>
+      </c>
+      <c r="F102" t="s">
+        <v>5</v>
+      </c>
+      <c r="G102" t="s">
+        <v>353</v>
+      </c>
+      <c r="H102" t="s">
+        <v>5</v>
+      </c>
+      <c r="I102" t="s">
+        <v>5</v>
+      </c>
+      <c r="K102" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11">
+      <c r="A103" t="s">
+        <v>18</v>
+      </c>
+      <c r="B103" t="s">
+        <v>354</v>
+      </c>
+      <c r="D103" t="s">
+        <v>355</v>
+      </c>
+      <c r="E103" t="s">
+        <v>356</v>
+      </c>
+      <c r="F103" t="s">
+        <v>5</v>
+      </c>
+      <c r="G103" t="s">
+        <v>357</v>
+      </c>
+      <c r="H103" t="s">
+        <v>5</v>
+      </c>
+      <c r="I103" t="s">
+        <v>5</v>
+      </c>
+      <c r="K103" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11">
+      <c r="A104" t="s">
+        <v>86</v>
+      </c>
+      <c r="B104" t="s">
+        <v>358</v>
+      </c>
+      <c r="D104" t="s">
+        <v>313</v>
+      </c>
+      <c r="E104" t="s">
+        <v>141</v>
+      </c>
+      <c r="F104" t="s">
+        <v>5</v>
+      </c>
+      <c r="G104" t="s">
+        <v>359</v>
+      </c>
+      <c r="H104" t="s">
+        <v>5</v>
+      </c>
+      <c r="I104" t="s">
+        <v>5</v>
+      </c>
+      <c r="K104" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11">
+      <c r="A105" t="s">
+        <v>86</v>
+      </c>
+      <c r="B105" t="s">
+        <v>360</v>
+      </c>
+      <c r="D105" t="s">
+        <v>361</v>
+      </c>
+      <c r="E105" t="s">
+        <v>147</v>
+      </c>
+      <c r="F105" t="s">
+        <v>5</v>
+      </c>
+      <c r="G105" t="s">
+        <v>362</v>
+      </c>
+      <c r="H105" t="s">
+        <v>5</v>
+      </c>
+      <c r="I105" t="s">
+        <v>5</v>
+      </c>
+      <c r="K105" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11">
+      <c r="A106" t="s">
+        <v>86</v>
+      </c>
+      <c r="B106" t="s">
+        <v>363</v>
+      </c>
+      <c r="D106" t="s">
+        <v>335</v>
+      </c>
+      <c r="E106" t="s">
+        <v>158</v>
+      </c>
+      <c r="F106" t="s">
+        <v>5</v>
+      </c>
+      <c r="G106" t="s">
+        <v>159</v>
+      </c>
+      <c r="H106" t="s">
+        <v>5</v>
+      </c>
+      <c r="I106" t="s">
+        <v>5</v>
+      </c>
+      <c r="K106" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11">
+      <c r="A107" t="s">
+        <v>86</v>
+      </c>
+      <c r="B107" t="s">
+        <v>332</v>
+      </c>
+      <c r="D107" t="s">
+        <v>340</v>
+      </c>
+      <c r="E107" t="s">
+        <v>164</v>
+      </c>
+      <c r="F107" t="s">
+        <v>5</v>
+      </c>
+      <c r="G107" t="s">
+        <v>169</v>
+      </c>
+      <c r="H107" t="s">
+        <v>5</v>
+      </c>
+      <c r="I107" t="s">
+        <v>5</v>
+      </c>
+      <c r="K107" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11">
+      <c r="A108" t="s">
+        <v>18</v>
+      </c>
+      <c r="B108" t="s">
+        <v>364</v>
+      </c>
+      <c r="D108" t="s">
+        <v>365</v>
+      </c>
+      <c r="E108" t="s">
+        <v>174</v>
+      </c>
+      <c r="F108" t="s">
+        <v>5</v>
+      </c>
+      <c r="G108" t="s">
+        <v>366</v>
+      </c>
+      <c r="H108" t="s">
+        <v>5</v>
+      </c>
+      <c r="I108" t="s">
+        <v>5</v>
+      </c>
+      <c r="K108" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11">
+      <c r="A110" t="s">
+        <v>18</v>
+      </c>
+      <c r="B110" t="s">
+        <v>368</v>
+      </c>
+      <c r="D110" t="s">
+        <v>337</v>
+      </c>
+      <c r="E110" t="s">
+        <v>369</v>
+      </c>
+      <c r="F110" t="s">
+        <v>5</v>
+      </c>
+      <c r="G110" t="s">
+        <v>370</v>
+      </c>
+      <c r="J110" t="s">
+        <v>5</v>
+      </c>
+      <c r="K110" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11">
+      <c r="A111" t="s">
+        <v>1</v>
+      </c>
+      <c r="B111" t="s">
+        <v>371</v>
+      </c>
+      <c r="D111" t="s">
+        <v>372</v>
+      </c>
+      <c r="E111" t="s">
+        <v>243</v>
+      </c>
+      <c r="F111" t="s">
+        <v>5</v>
+      </c>
+      <c r="G111" t="s">
+        <v>373</v>
+      </c>
+      <c r="J111" t="s">
+        <v>5</v>
+      </c>
+      <c r="K111" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11">
+      <c r="A112" t="s">
+        <v>1</v>
+      </c>
+      <c r="B112" t="s">
+        <v>374</v>
+      </c>
+      <c r="D112" t="s">
+        <v>328</v>
+      </c>
+      <c r="E112" t="s">
+        <v>268</v>
+      </c>
+      <c r="F112" t="s">
+        <v>5</v>
+      </c>
+      <c r="G112" t="s">
+        <v>375</v>
+      </c>
+      <c r="J112" t="s">
+        <v>5</v>
+      </c>
+      <c r="K112" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11">
+      <c r="A113" t="s">
+        <v>86</v>
+      </c>
+      <c r="B113" t="s">
+        <v>376</v>
+      </c>
+      <c r="D113" t="s">
+        <v>361</v>
+      </c>
+      <c r="E113" t="s">
+        <v>258</v>
+      </c>
+      <c r="F113" t="s">
+        <v>5</v>
+      </c>
+      <c r="G113" t="s">
+        <v>377</v>
+      </c>
+      <c r="H113" t="s">
+        <v>74</v>
+      </c>
+      <c r="J113" t="s">
+        <v>5</v>
+      </c>
+      <c r="K113" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11">
+      <c r="A114" t="s">
+        <v>37</v>
+      </c>
+      <c r="B114" t="s">
+        <v>378</v>
+      </c>
+      <c r="D114" t="s">
+        <v>352</v>
+      </c>
+      <c r="E114" t="s">
+        <v>379</v>
+      </c>
+      <c r="G114" t="s">
+        <v>380</v>
+      </c>
+      <c r="H114" t="s">
+        <v>5</v>
+      </c>
+      <c r="J114" t="s">
+        <v>5</v>
+      </c>
+      <c r="K114" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:L57">
     <sortCondition ref="E2:E57"/>

</xml_diff>